<commit_message>
added new test case in the loginTest class
</commit_message>
<xml_diff>
--- a/src/test/resources/LoginDetails.xlsx
+++ b/src/test/resources/LoginDetails.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Practice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Practice\BankAutomationFrameWork\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E30535E5-7DF6-48D2-89D8-A85F67167314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D5E36A-3400-48FF-AEC1-EBA93DECBA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{88F985B6-C966-476F-97F7-DB362E5F5916}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Username</t>
   </si>
@@ -59,6 +59,18 @@
   </si>
   <si>
     <t>pass3</t>
+  </si>
+  <si>
+    <t>shiva</t>
+  </si>
+  <si>
+    <t>shiva123</t>
+  </si>
+  <si>
+    <t>sri</t>
+  </si>
+  <si>
+    <t>sri123</t>
   </si>
 </sst>
 </file>
@@ -419,7 +431,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,7 +459,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B38A4423-B19C-46D7-A413-9FACFAFB49FC}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -487,6 +499,22 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>